<commit_message>
Wrote code to compile sulfide plates for May 2025, combine with metadata, and visualize data
</commit_message>
<xml_diff>
--- a/Porewater/Sulfide/Synoptic_CB/2025/May/Raw Data/20250529_COMPASS_H2S_IDs.xlsx
+++ b/Porewater/Sulfide/Synoptic_CB/2025/May/Raw Data/20250529_COMPASS_H2S_IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/readz_si_edu1/Documents/synoptic-discrete-data/Porewater/Sulfide/Synoptic_CB/2025/May/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{3840606C-6908-43EA-8BEB-0E3170A8FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5291D134-B01C-4C52-9971-173980BD24CD}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{3840606C-6908-43EA-8BEB-0E3170A8FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8647B22E-8568-4BAD-802B-CE3B6156C2BC}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{8DBD12CC-0278-4D7F-B40A-7CBDE2522597}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COMPASS_Synoptic_CB_MonMon_2025!$A$1:$A$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COMPASS_Synoptic_CB_MonMon_2025!$A$2:$A$126</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">COMPASS_Synoptic_CB_MonMon_2025!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="24">
   <si>
     <t>GCW</t>
   </si>
@@ -104,6 +104,24 @@
   <si>
     <t>SWAMP</t>
   </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Replicate</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
 </sst>
 </file>
 
@@ -156,6 +174,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925E985A-FED3-4128-81D0-4F8068FB988C}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,28 +509,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>202505</v>
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -523,12 +545,12 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -540,15 +562,15 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -563,12 +585,12 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -580,15 +602,15 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -603,12 +625,12 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -617,10 +639,10 @@
         <v>202505</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -628,7 +650,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -643,12 +665,12 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -660,15 +682,15 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -683,12 +705,12 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -703,12 +725,12 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -720,15 +742,15 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -743,12 +765,12 @@
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -763,12 +785,12 @@
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -777,18 +799,18 @@
         <v>202505</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -803,12 +825,12 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -823,12 +845,12 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -840,15 +862,15 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -863,12 +885,12 @@
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -883,12 +905,12 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -900,15 +922,15 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -923,12 +945,12 @@
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -937,15 +959,18 @@
         <v>202505</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -957,12 +982,12 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -974,32 +999,29 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>202505</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -1014,12 +1036,12 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
@@ -1031,15 +1053,15 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>14</v>
@@ -1054,12 +1076,12 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
@@ -1074,12 +1096,12 @@
         <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>14</v>
@@ -1091,15 +1113,15 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
@@ -1114,12 +1136,12 @@
         <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -1134,12 +1156,12 @@
         <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>14</v>
@@ -1148,18 +1170,18 @@
         <v>202505</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>14</v>
@@ -1174,12 +1196,12 @@
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
@@ -1194,12 +1216,12 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>14</v>
@@ -1211,15 +1233,15 @@
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
@@ -1234,12 +1256,12 @@
         <v>5</v>
       </c>
       <c r="F38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -1254,12 +1276,12 @@
         <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -1271,15 +1293,15 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -1294,12 +1316,12 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
@@ -1308,18 +1330,18 @@
         <v>202505</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -1334,12 +1356,12 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>14</v>
@@ -1354,12 +1376,12 @@
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>14</v>
@@ -1371,15 +1393,15 @@
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
@@ -1394,12 +1416,12 @@
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>14</v>
@@ -1411,15 +1433,15 @@
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>14</v>
@@ -1434,12 +1456,12 @@
         <v>6</v>
       </c>
       <c r="F48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>14</v>
@@ -1454,12 +1476,12 @@
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>14</v>
@@ -1468,15 +1490,18 @@
         <v>202505</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -1488,12 +1513,12 @@
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
@@ -1505,32 +1530,29 @@
         <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C53">
         <v>202505</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E53" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>15</v>
@@ -1545,12 +1567,12 @@
         <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
@@ -1565,12 +1587,12 @@
         <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>15</v>
@@ -1582,15 +1604,15 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
@@ -1605,12 +1627,12 @@
         <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
@@ -1625,12 +1647,12 @@
         <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -1642,15 +1664,15 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -1659,18 +1681,18 @@
         <v>202505</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F60" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
@@ -1685,12 +1707,12 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>15</v>
@@ -1702,15 +1724,15 @@
         <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>15</v>
@@ -1725,12 +1747,12 @@
         <v>5</v>
       </c>
       <c r="F63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>15</v>
@@ -1745,12 +1767,12 @@
         <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>
@@ -1762,15 +1784,15 @@
         <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>15</v>
@@ -1785,12 +1807,12 @@
         <v>6</v>
       </c>
       <c r="F66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>15</v>
@@ -1799,18 +1821,18 @@
         <v>202505</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E67" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>15</v>
@@ -1825,12 +1847,12 @@
         <v>2</v>
       </c>
       <c r="F68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>15</v>
@@ -1845,12 +1867,12 @@
         <v>2</v>
       </c>
       <c r="F69" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
@@ -1862,15 +1884,15 @@
         <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>15</v>
@@ -1885,12 +1907,12 @@
         <v>5</v>
       </c>
       <c r="F71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>15</v>
@@ -1905,12 +1927,12 @@
         <v>5</v>
       </c>
       <c r="F72" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>15</v>
@@ -1922,15 +1944,15 @@
         <v>9</v>
       </c>
       <c r="E73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>15</v>
@@ -1939,15 +1961,18 @@
         <v>202505</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="F74" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>15</v>
@@ -1959,12 +1984,12 @@
         <v>10</v>
       </c>
       <c r="E75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>15</v>
@@ -1976,32 +2001,29 @@
         <v>10</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C77">
         <v>202505</v>
       </c>
       <c r="D77" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E77" t="s">
-        <v>2</v>
-      </c>
-      <c r="F77" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>16</v>
@@ -2016,12 +2038,12 @@
         <v>2</v>
       </c>
       <c r="F78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
@@ -2036,12 +2058,12 @@
         <v>2</v>
       </c>
       <c r="F79" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>16</v>
@@ -2053,15 +2075,15 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F80" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>16</v>
@@ -2076,12 +2098,12 @@
         <v>5</v>
       </c>
       <c r="F81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>16</v>
@@ -2096,12 +2118,12 @@
         <v>5</v>
       </c>
       <c r="F82" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>16</v>
@@ -2113,15 +2135,15 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>16</v>
@@ -2136,12 +2158,12 @@
         <v>6</v>
       </c>
       <c r="F84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>16</v>
@@ -2156,12 +2178,12 @@
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>16</v>
@@ -2170,18 +2192,18 @@
         <v>202505</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F86" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>16</v>
@@ -2196,12 +2218,12 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>16</v>
@@ -2216,12 +2238,12 @@
         <v>2</v>
       </c>
       <c r="F88" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>16</v>
@@ -2233,15 +2255,15 @@
         <v>17</v>
       </c>
       <c r="E89" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F89" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>16</v>
@@ -2256,12 +2278,12 @@
         <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>16</v>
@@ -2276,12 +2298,12 @@
         <v>5</v>
       </c>
       <c r="F91" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>16</v>
@@ -2293,15 +2315,15 @@
         <v>17</v>
       </c>
       <c r="E92" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>16</v>
@@ -2316,12 +2338,12 @@
         <v>6</v>
       </c>
       <c r="F93" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>16</v>
@@ -2336,12 +2358,12 @@
         <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>16</v>
@@ -2350,18 +2372,18 @@
         <v>202505</v>
       </c>
       <c r="D95" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E95" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F95" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>16</v>
@@ -2376,12 +2398,12 @@
         <v>2</v>
       </c>
       <c r="F96" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>16</v>
@@ -2396,12 +2418,12 @@
         <v>2</v>
       </c>
       <c r="F97" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>16</v>
@@ -2413,15 +2435,15 @@
         <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F98" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>16</v>
@@ -2436,12 +2458,12 @@
         <v>5</v>
       </c>
       <c r="F99" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>16</v>
@@ -2456,12 +2478,12 @@
         <v>5</v>
       </c>
       <c r="F100" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>16</v>
@@ -2473,15 +2495,15 @@
         <v>7</v>
       </c>
       <c r="E101" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F101" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>16</v>
@@ -2496,12 +2518,12 @@
         <v>6</v>
       </c>
       <c r="F102" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>16</v>
@@ -2516,12 +2538,12 @@
         <v>6</v>
       </c>
       <c r="F103" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
         <v>16</v>
@@ -2530,18 +2552,18 @@
         <v>202505</v>
       </c>
       <c r="D104" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E104" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F104" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
         <v>16</v>
@@ -2556,12 +2578,12 @@
         <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
         <v>16</v>
@@ -2576,12 +2598,12 @@
         <v>2</v>
       </c>
       <c r="F106" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
         <v>16</v>
@@ -2593,15 +2615,15 @@
         <v>9</v>
       </c>
       <c r="E107" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F107" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>16</v>
@@ -2616,12 +2638,12 @@
         <v>5</v>
       </c>
       <c r="F108" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
         <v>16</v>
@@ -2636,12 +2658,12 @@
         <v>5</v>
       </c>
       <c r="F109" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
         <v>16</v>
@@ -2653,15 +2675,15 @@
         <v>9</v>
       </c>
       <c r="E110" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F110" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
         <v>16</v>
@@ -2676,49 +2698,52 @@
         <v>6</v>
       </c>
       <c r="F111" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>16</v>
+      </c>
+      <c r="C112">
+        <v>202505</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" t="s">
+        <v>6</v>
+      </c>
+      <c r="F112" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113" s="1">
         <v>112</v>
       </c>
-      <c r="B112" t="s">
-        <v>16</v>
-      </c>
-      <c r="C112">
-        <v>202505</v>
-      </c>
-      <c r="D112" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" t="s">
-        <v>6</v>
-      </c>
-      <c r="F112" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A113" s="1">
+      <c r="B113" t="s">
+        <v>16</v>
+      </c>
+      <c r="C113">
+        <v>202505</v>
+      </c>
+      <c r="D113" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" t="s">
+        <v>6</v>
+      </c>
+      <c r="F113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114" s="1">
         <v>113</v>
-      </c>
-      <c r="B113" t="s">
-        <v>16</v>
-      </c>
-      <c r="C113">
-        <v>202505</v>
-      </c>
-      <c r="D113" t="s">
-        <v>10</v>
-      </c>
-      <c r="E113" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" s="1">
-        <v>114</v>
       </c>
       <c r="B114" t="s">
         <v>16</v>
@@ -2730,12 +2755,12 @@
         <v>10</v>
       </c>
       <c r="E114" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>16</v>
@@ -2747,23 +2772,40 @@
         <v>10</v>
       </c>
       <c r="E115" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>16</v>
+      </c>
+      <c r="C116">
+        <v>202505</v>
+      </c>
+      <c r="D116" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A116" s="1"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="1"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>